<commit_message>
Update 2020-02-11 - 2020-03-10.xlsx
</commit_message>
<xml_diff>
--- a/2020-02-11 - 2020-03-10.xlsx
+++ b/2020-02-11 - 2020-03-10.xlsx
@@ -247,13 +247,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51:G51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,58 +651,58 @@
       <c r="B9" s="3">
         <v>43872</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -711,58 +711,58 @@
       <c r="B16" s="3">
         <v>43873</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -771,40 +771,40 @@
       <c r="B23" s="3">
         <v>43874</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -813,49 +813,49 @@
       <c r="B28" s="3">
         <v>43875</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -864,40 +864,40 @@
       <c r="B34" s="3">
         <v>43878</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -906,31 +906,31 @@
       <c r="B39" s="3">
         <v>43879</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -939,22 +939,22 @@
       <c r="B43" s="3">
         <v>43880</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -963,31 +963,31 @@
       <c r="B46" s="3">
         <v>43881</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
@@ -996,40 +996,40 @@
       <c r="B50" s="3">
         <v>43882</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -1038,22 +1038,22 @@
       <c r="B55" s="3">
         <v>43887</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -1062,31 +1062,31 @@
       <c r="B58" s="3">
         <v>43888</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
@@ -1095,22 +1095,22 @@
       <c r="B62" s="3">
         <v>43889</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
@@ -1119,22 +1119,22 @@
       <c r="B65" s="3">
         <v>43893</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
@@ -1143,22 +1143,22 @@
       <c r="B68" s="3">
         <v>43894</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
@@ -1167,22 +1167,22 @@
       <c r="B71" s="3">
         <v>43895</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
@@ -1191,31 +1191,31 @@
       <c r="B74" s="3">
         <v>43896</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="6" t="s">
+      <c r="C75" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
@@ -1224,22 +1224,22 @@
       <c r="B78" s="3">
         <v>43899</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C78" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="7" t="s">
+      <c r="C79" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
@@ -1248,35 +1248,74 @@
       <c r="B81" s="3">
         <v>43900</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C81" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="7" t="s">
+      <c r="C82" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C82:G82"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="C81:G81"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="C68:G68"/>
+    <mergeCell ref="C66:G66"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="C65:G65"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="C59:G59"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C23:G23"/>
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C16:G16"/>
@@ -1285,55 +1324,16 @@
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="C58:G58"/>
-    <mergeCell ref="C59:G59"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="C68:G68"/>
-    <mergeCell ref="C66:G66"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="C65:G65"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="C62:G62"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="C74:G74"/>
-    <mergeCell ref="C75:G75"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="C82:G82"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="C81:G81"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C14:G14" r:id="rId1" display="link : https://github.com/alpinnz/PKL/tree/master/2020-02-11%20-%202020-03-10/2020-02-11"/>

</xml_diff>